<commit_message>
Various fixes catering for missing or incorrect data
</commit_message>
<xml_diff>
--- a/resources/cosmed_fields.xlsx
+++ b/resources/cosmed_fields.xlsx
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -720,9 +720,6 @@
     <t>rq</t>
   </si>
   <si>
-    <t xml:space="preserve">hr </t>
-  </si>
-  <si>
     <t>sbp</t>
   </si>
   <si>
@@ -781,6 +778,9 @@
   </si>
   <si>
     <t>AxD</t>
+  </si>
+  <si>
+    <t>hr</t>
   </si>
 </sst>
 </file>
@@ -2103,7 +2103,7 @@
         <v>198</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I30">
         <f>[1]Data!$X$45-[1]Data!$X$47</f>
@@ -2133,7 +2133,7 @@
         <v>201</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I31">
         <f>[1]Data!$X$45-[1]Data!$X$51</f>
@@ -2163,7 +2163,7 @@
         <v>204</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I32">
         <f>[1]Data!$X$45-[1]Data!$X$55</f>
@@ -2181,7 +2181,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>27</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>28</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
@@ -2295,7 +2295,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>89</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>90</v>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>193</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>196</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>199</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>202</v>
@@ -3140,37 +3140,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
@@ -3180,17 +3180,17 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
@@ -3200,17 +3200,17 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
@@ -3220,17 +3220,17 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added integer fields check for XNAT
</commit_message>
<xml_diff>
--- a/resources/cosmed_fields.xlsx
+++ b/resources/cosmed_fields.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="250">
   <si>
     <t>VT</t>
   </si>
@@ -781,6 +781,9 @@
   </si>
   <si>
     <t>hr</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -2178,183 +2181,247 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C19" sqref="C19:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>205</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>145</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>223</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>224</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>225</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>209</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>226</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>227</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>248</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>228</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>229</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>230</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>231</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>232</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>210</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>211</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>233</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>234</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>235</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>236</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>202</v>
+      </c>
+      <c r="C21" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>